<commit_message>
Fix cost swing weighting
</commit_message>
<xml_diff>
--- a/app/data/Rubric.xlsx
+++ b/app/data/Rubric.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric v3" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Definitions" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Definitions old" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Rubric v1" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Cost_Model" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="373">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -1286,15 +1287,47 @@
   <si>
     <t xml:space="preserve">Has data collection tools. For example, can use the mobile app to record and then import into MAXQDA.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual Lease for User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$$$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiuser</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="\$#,##0_);[RED]&quot;($&quot;#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1381,6 +1414,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1424,13 +1464,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1489,6 +1531,18 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1578,19 +1632,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,20 +2478,20 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,11 +3426,14 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
@@ -3919,7 +3976,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4606,19 +4663,19 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5650,4 +5707,159 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="16" t="n">
+        <v>370</v>
+      </c>
+      <c r="C2" s="17" t="n">
+        <f aca="false">(B$5-B2)/(B$5-B$7)</f>
+        <v>0.328493647912886</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="16" t="n">
+        <v>139</v>
+      </c>
+      <c r="C3" s="17" t="n">
+        <f aca="false">(B$5-B3)/(B$5-B$7)</f>
+        <v>0.747731397459165</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="16" t="n">
+        <v>202</v>
+      </c>
+      <c r="C4" s="17" t="n">
+        <f aca="false">(B$5-B4)/(B$5-B$7)</f>
+        <v>0.633393829401089</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16" t="n">
+        <v>551</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <f aca="false">(B$5-B5)/(B$5-B$7)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="16" t="n">
+        <v>379</v>
+      </c>
+      <c r="C6" s="17" t="n">
+        <f aca="false">(B$5-B6)/(B$5-B$7)</f>
+        <v>0.312159709618875</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17" t="n">
+        <f aca="false">(B$5-B7)/(B$5-B$7)</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="16" t="n">
+        <v>119</v>
+      </c>
+      <c r="C8" s="17" t="n">
+        <f aca="false">(B$5-B8)/(B$5-B$7)</f>
+        <v>0.784029038112523</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>